<commit_message>
Updating the supplementary data (tables)
</commit_message>
<xml_diff>
--- a/tables/DataS2.xlsx
+++ b/tables/DataS2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\Documents\Artigo Extincao na MA\data analysis\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF0B0E-98D2-4B7A-97A4-67343635B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDB23B7-B005-48FC-9C39-5EF0E0C96233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="784" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="784" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="empirical GenLength for plants" sheetId="3" r:id="rId1"/>
@@ -3128,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H146"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8980,7 +8980,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="P24" sqref="P24"/>
       <selection pane="topRight" activeCell="P24" sqref="P24"/>
       <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
@@ -13056,8 +13056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>